<commit_message>
defined sphere colors in 3D localization
</commit_message>
<xml_diff>
--- a/3D/coords.xlsx
+++ b/3D/coords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\localization\3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8DD2DC-8B60-42CF-9F00-F6A5B7CF9BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5293666-B3CE-460D-AE6E-CE5C49EBE3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -706,6 +706,9 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
       <c r="B4" s="7">
         <v>7</v>
       </c>
@@ -769,6 +772,9 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -829,6 +835,74 @@
       <c r="T5" s="12">
         <f>SQRT((Q5-$B5)^2+(R5-$C5)^2+(S5-$D5)^2)</f>
         <v>6.7082039324993694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <f>SQRT((E6-$B6)^2+(F6-$C6)^2+(G6-$D6)^2)</f>
+        <v>8.7749643873921226</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>10</v>
+      </c>
+      <c r="K6" s="9">
+        <f>10/3</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="L6" s="9">
+        <f>SQRT((I6-$B6)^2+(J6-$C6)^2+(K6-$D6)^2)</f>
+        <v>5.8972686709847109</v>
+      </c>
+      <c r="M6" s="10">
+        <v>10</v>
+      </c>
+      <c r="N6" s="10">
+        <v>10</v>
+      </c>
+      <c r="O6" s="10">
+        <f>2*(10/3)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="P6" s="10">
+        <f>SQRT((M6-$B6)^2+(N6-$C6)^2+(O6-$D6)^2)</f>
+        <v>7.4012011037248389</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>10</v>
+      </c>
+      <c r="R6" s="12">
+        <v>0</v>
+      </c>
+      <c r="S6" s="12">
+        <v>10</v>
+      </c>
+      <c r="T6" s="12">
+        <f>SQRT((Q6-$B6)^2+(R6-$C6)^2+(S6-$D6)^2)</f>
+        <v>9.8488578017961039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed color of intersection point from black to red
</commit_message>
<xml_diff>
--- a/3D/coords.xlsx
+++ b/3D/coords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\localization\3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5293666-B3CE-460D-AE6E-CE5C49EBE3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBDDCCD-8BB6-4DC1-B225-B3246E562127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,26 +492,26 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.83984375" style="7"/>
-    <col min="5" max="6" width="9.15625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.15625" style="8" customWidth="1"/>
-    <col min="9" max="10" width="9.15625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.68359375" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.68359375" style="9" customWidth="1"/>
-    <col min="13" max="14" width="9.15625" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.68359375" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.68359375" style="10" customWidth="1"/>
-    <col min="17" max="18" width="9.15625" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.68359375" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.68359375" style="12" customWidth="1"/>
+    <col min="1" max="4" width="8.85546875" style="7"/>
+    <col min="5" max="6" width="9.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="8" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="9" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="10" customWidth="1"/>
+    <col min="17" max="18" width="9.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -573,7 +573,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -639,7 +639,7 @@
         <v>4.358898943540674</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -705,7 +705,7 @@
         <v>7.0710678118654755</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -771,7 +771,7 @@
         <v>8.3066238629180749</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -837,7 +837,7 @@
         <v>6.7082039324993694</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>

</xml_diff>